<commit_message>
update current stock level report and it's lib file
</commit_message>
<xml_diff>
--- a/Library/BillingReportsTestScripts_ExecutionResult_LPHV2.1.8C.xlsx
+++ b/Library/BillingReportsTestScripts_ExecutionResult_LPHV2.1.8C.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>TC007</t>
+  </si>
+  <si>
+    <t>Report not visible for FO</t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,12 +578,14 @@
         <v>10</v>
       </c>
       <c r="D4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
@@ -621,12 +626,14 @@
         <v>10</v>
       </c>
       <c r="D6" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
@@ -670,12 +677,14 @@
         <v>10</v>
       </c>
       <c r="D8" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G8" s="5" t="s">
         <v>9</v>
       </c>
@@ -685,6 +694,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>